<commit_message>
add grass lod + bush lod
</commit_message>
<xml_diff>
--- a/Docs/Bench/BenchPerf270323.xlsx
+++ b/Docs/Bench/BenchPerf270323.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UnityDev\Proj\DorianDeVillele\Docs\Bench\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F8591B-ABFA-4720-874A-924296F66612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F89790-3E0A-401A-8DA8-5CD1186E8A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{300C4252-A5F4-4E16-A14B-563A41E9AEA8}"/>
   </bookViews>
@@ -425,7 +425,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A1D2283-66F6-4059-AA6C-3B7183D11099}">
   <dimension ref="B4:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>